<commit_message>
cree base agregada, faltan detalles. no guarde aun. revise encuestas posibles de descarga
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/unique_candidates_tomerge_incompletos_completado.xlsx
+++ b/tesis_doctorado/datav2023/unique_candidates_tomerge_incompletos_completado.xlsx
@@ -142,7 +142,7 @@
     <t xml:space="preserve">Andrés Manuel López Obrador</t>
   </si>
   <si>
-    <t xml:space="preserve">Jaime Rodriguez Calderon</t>
+    <t xml:space="preserve">Felipe Calderon</t>
   </si>
   <si>
     <t xml:space="preserve">Roberto Madrazo</t>
@@ -221,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -251,12 +251,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -324,11 +318,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,8 +405,8 @@
   </sheetPr>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>